<commit_message>
Added a new pattern to underground levels that is based upon a pattern from underwater level types
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Supported ROMs.xlsx
+++ b/SMB1/Research Docs/Supported ROMs.xlsx
@@ -45,9 +45,6 @@
     <t>FDS</t>
   </si>
   <si>
-    <t>Super Mario Bros (J).FDS</t>
-  </si>
-  <si>
     <t>Super Mario Bros. + Duck Hunt (U).nes</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>0E198DF9E0D5863F865838EAFF7090596DA548D95CE9CDA8BFBBAF0DC3E6591104140924C1107464CCEE547DA82301E615F1E7B33FB38CE3705B64B5531060D8</t>
+  </si>
+  <si>
+    <t>Super Mario Bros. (J).fds</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +484,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -495,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -503,13 +503,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -517,16 +517,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -537,10 +537,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,18 +548,18 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -578,58 +578,58 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Supported ROMs spreadsheet
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Supported ROMs.xlsx
+++ b/SMB1/Research Docs/Supported ROMs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>SHA-2 (512 bit) Checksum</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Super Mario Bros. + Duck Hunt (E).nes</t>
   </si>
   <si>
-    <t>Super Mario Bros. + Tetris + Nintendo World Cup (E) [!].nes</t>
-  </si>
-  <si>
     <t>DUCK</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>DUCK-E</t>
   </si>
   <si>
-    <t>TETRIS</t>
-  </si>
-  <si>
     <t>USA-0</t>
   </si>
   <si>
@@ -121,12 +115,6 @@
   </si>
   <si>
     <t>2EA868BEAF5F4FE99E9F7FAF8A602450</t>
-  </si>
-  <si>
-    <t>20A38E902CBC051D389E78D260AF7D45</t>
-  </si>
-  <si>
-    <t>0E198DF9E0D5863F865838EAFF7090596DA548D95CE9CDA8BFBBAF0DC3E6591104140924C1107464CCEE547DA82301E615F1E7B33FB38CE3705B64B5531060D8</t>
   </si>
   <si>
     <t>Super Mario Bros. (J).fds</t>
@@ -468,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -503,13 +491,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -517,16 +505,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -537,10 +525,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,13 +536,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -570,7 +558,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -578,58 +566,44 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dropped support for bad ROM dumps
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Supported ROMs.xlsx
+++ b/SMB1/Research Docs/Supported ROMs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>SHA-2 (512 bit) Checksum</t>
   </si>
@@ -57,18 +57,12 @@
     <t>Super Mario Bros. + Duck Hunt + World Class Track Meet (U).nes</t>
   </si>
   <si>
-    <t>Super Mario Bros. + Duck Hunt (E).nes</t>
-  </si>
-  <si>
     <t>DUCK</t>
   </si>
   <si>
     <t>TRACK</t>
   </si>
   <si>
-    <t>DUCK-E</t>
-  </si>
-  <si>
     <t>USA-0</t>
   </si>
   <si>
@@ -109,12 +103,6 @@
   </si>
   <si>
     <t>7815F5BD6568AE3E2FB428CEA510415FE688971A40AF2E9D354E37AC0D3B98E74F53A8F9BD9A7FBF1785A3B785EF447B5D770F3DE77D21E4B063FC7B5D7DA5EF</t>
-  </si>
-  <si>
-    <t>01F8DAC3E8281C93A758355D0FC9618ED5239B224650BE9241F04CB8231EB3D07D8F6D59CBF3AC24D1D55CB008D7F71F8F76B6630D3DF739265EC4B477D49670</t>
-  </si>
-  <si>
-    <t>2EA868BEAF5F4FE99E9F7FAF8A602450</t>
   </si>
   <si>
     <t>Super Mario Bros. (J).fds</t>
@@ -456,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -491,13 +479,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -505,16 +493,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -525,10 +513,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -536,13 +524,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -558,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -566,44 +554,30 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>